<commit_message>
added result calculation and saving
</commit_message>
<xml_diff>
--- a/questions_template.xlsx
+++ b/questions_template.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sagunkarki/Desktop/survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ED9EAB-F439-B543-ADB7-D360B8D8862D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59119E2C-7EA5-3C4E-9326-C8BA8334DB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questions" sheetId="1" r:id="rId1"/>
-    <sheet name="details" sheetId="2" r:id="rId2"/>
-    <sheet name="result" sheetId="3" r:id="rId3"/>
-    <sheet name="abbrevations" sheetId="4" r:id="rId4"/>
+    <sheet name="result" sheetId="3" r:id="rId2"/>
+    <sheet name="abbrevations" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="220">
   <si>
     <t>cbq_num</t>
   </si>
@@ -693,27 +692,6 @@
   </si>
   <si>
     <t>Has a hard time concentrating on an activity when there are distracting noises.</t>
-  </si>
-  <si>
-    <t>details</t>
-  </si>
-  <si>
-    <t>values</t>
-  </si>
-  <si>
-    <t>survey_id</t>
-  </si>
-  <si>
-    <t>data_entered_by</t>
-  </si>
-  <si>
-    <t>first_data_entry_date</t>
-  </si>
-  <si>
-    <t>verifying_data_entry_date</t>
-  </si>
-  <si>
-    <t>first_data_is_equals_to_second_entry</t>
   </si>
   <si>
     <t>short_form</t>
@@ -755,18 +733,12 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -781,12 +753,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -910,17 +881,6 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D430D427-27FB-2E4A-BD00-20186C313C0B}" name="Table3" displayName="Table3" ref="A1:B1048576" totalsRowShown="0">
-  <autoFilter ref="A1:B1048576" xr:uid="{D430D427-27FB-2E4A-BD00-20186C313C0B}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{4E9BE0C0-5AC5-2640-A7D6-8207B9CB1517}" name="details"/>
-    <tableColumn id="2" xr3:uid="{B05F2692-BDC7-4C48-8BB5-6554B90C19C2}" name="values"/>
-  </tableColumns>
-  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DC43ED70-553B-1349-951D-A776EA76960F}" name="Table5" displayName="Table5" ref="A1:B1048576" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
   <autoFilter ref="A1:B1048576" xr:uid="{DC43ED70-553B-1349-951D-A776EA76960F}"/>
   <tableColumns count="2">
@@ -1218,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E196"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1257,9 +1217,6 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -1271,9 +1228,6 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -1284,9 +1238,6 @@
       </c>
       <c r="D4" t="s">
         <v>10</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -3635,67 +3586,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9881B8-3B1C-DA48-96E9-70F3F9A19D8B}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA2C4AE-66F7-7241-9272-480D26122344}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
@@ -3703,83 +3599,83 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7984BD27-6509-4349-8307-6D75B409016C}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="12.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>226</v>
+      <c r="A1" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
+      <c r="A2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
+      <c r="A3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
+      <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
+      <c r="A5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
+      <c r="A6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
+      <c r="A7" s="2"/>
     </row>
     <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
+      <c r="A8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
+      <c r="A9" s="2"/>
     </row>
     <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
+      <c r="A10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
+      <c r="A11" s="2"/>
     </row>
     <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="A12" s="2"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
+      <c r="A13" s="2"/>
     </row>
     <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
+      <c r="A14" s="2"/>
     </row>
     <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
+      <c r="A15" s="2"/>
     </row>
     <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
+      <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
+      <c r="A17" s="2"/>
     </row>
     <row r="18" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
+      <c r="A18" s="2"/>
     </row>
     <row r="19" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
+      <c r="A19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>